<commit_message>
Removed ROM loader idea from architecture
</commit_message>
<xml_diff>
--- a/Instructions_T-States.xlsx
+++ b/Instructions_T-States.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\TTL-Computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3044B10B-7E6C-437A-BF62-D5704CA81694}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C77557E1-D853-4D9D-9A78-777D69109318}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="2" xr2:uid="{3D2DD9FF-2996-4470-A4B6-A8539109D178}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1" xr2:uid="{3D2DD9FF-2996-4470-A4B6-A8539109D178}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Control lines" sheetId="2" r:id="rId2"/>
     <sheet name="T-states" sheetId="3" r:id="rId3"/>
+    <sheet name="ROM Loader" sheetId="4" r:id="rId4"/>
+    <sheet name="Notes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="222">
   <si>
     <t>Opcode</t>
   </si>
@@ -628,10 +630,658 @@
   </si>
   <si>
     <r>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OUT</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <r>
+      <t>SEQ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>res</t>
+    </r>
+  </si>
+  <si>
+    <t>Load PC into MAR</t>
+  </si>
+  <si>
+    <t>Increment PC</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inc</t>
+    </r>
+  </si>
+  <si>
+    <t>Load RAM byte (high) into Y, incr PC</t>
+  </si>
+  <si>
+    <t>Load OpCode from RAM, incr PC</t>
+  </si>
+  <si>
+    <t>Load RAM byte (low) into X, incr PC</t>
+  </si>
+  <si>
+    <t>Load X &amp; Y into MAR</t>
+  </si>
+  <si>
+    <t>Load data from memory location into B and store A + B in A register</t>
+  </si>
+  <si>
+    <t>Load PC into X &amp; Y</t>
+  </si>
+  <si>
+    <t>Decrement PC</t>
+  </si>
+  <si>
+    <t>Load RAM byte (low) into X</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STK-in</t>
+    </r>
+  </si>
+  <si>
+    <t>Load Y (high addr) into RAM, incr SP</t>
+  </si>
+  <si>
+    <t>Load SP into MAR</t>
+  </si>
+  <si>
+    <r>
+      <t>STK</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>STK</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inc</t>
+    </r>
+  </si>
+  <si>
+    <t>Decrement SP</t>
+  </si>
+  <si>
+    <t>Load RAM byte (low) into X, decr SP</t>
+  </si>
+  <si>
+    <t>Load RAM byte (high) into Y</t>
+  </si>
+  <si>
+    <r>
+      <t>CLK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hlt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>RAM</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
@@ -644,10 +1294,198 @@
   </si>
   <si>
     <r>
-      <t>IN</t>
-    </r>
-    <r>
-      <rPr>
+      <t>OUT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>STK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>STK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STK-in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
@@ -660,10 +1498,79 @@
   </si>
   <si>
     <r>
-      <t>OUT</t>
-    </r>
-    <r>
-      <rPr>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ALU</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
@@ -676,90 +1583,164 @@
   </si>
   <si>
     <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PC-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SEQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>res</t>
+    </r>
+  </si>
+  <si>
+    <t>Load X (high addr) into RAM, incr SP, decr PC</t>
+  </si>
+  <si>
+    <t>Load X &amp; Y into PC, reset Sequencer</t>
+  </si>
+  <si>
+    <t>ALU Add (A+B), load ALU into A, load Flags, reset Sequencer</t>
+  </si>
+  <si>
+    <t>Load A into RAM, reset Sequencer</t>
+  </si>
+  <si>
+    <t>Load RAM byte into A, reset Sequencer</t>
+  </si>
+  <si>
+    <t>Load RAM byte into A, incr PC, reset SEQ</t>
+  </si>
+  <si>
+    <t>Load A into B, reset Sequencer</t>
+  </si>
+  <si>
+    <t>Run computer flag = 0</t>
+  </si>
+  <si>
+    <t>Internal counter = 0 (16-bit counter)</t>
+  </si>
+  <si>
+    <t>ROM address = counter</t>
+  </si>
+  <si>
+    <t>RAM address = counter</t>
+  </si>
+  <si>
+    <t>ROM out to RAM in</t>
+  </si>
+  <si>
+    <t>Pulse RAM write</t>
+  </si>
+  <si>
+    <t>Increase internal counter</t>
+  </si>
+  <si>
+    <t>Carry out counter = HALT</t>
+  </si>
+  <si>
+    <t>(clock + last carry out) -&gt; NOR -&gt; = clock for counter</t>
+  </si>
+  <si>
+    <t>last carry out = Run computer flag</t>
+  </si>
+  <si>
+    <t>Need microticks for this logic</t>
+  </si>
+  <si>
+    <t>4x binary counter</t>
+  </si>
+  <si>
+    <t>1x decade counter (microticks)</t>
+  </si>
+  <si>
+    <t>Pulse RAM Write</t>
+  </si>
+  <si>
+    <t>Increase counter</t>
+  </si>
+  <si>
+    <t>T0 = clock</t>
+  </si>
+  <si>
+    <t>T1 = inverted clock?</t>
+  </si>
+  <si>
+    <t>Use just 12 bits? = 4 kB ROM data</t>
+  </si>
+  <si>
+    <t>ROM/RAM</t>
+  </si>
+  <si>
+    <t>Toggle switch to boot from ROM</t>
+  </si>
+  <si>
+    <t>$0000-$3FFF = ROM (16 kB)</t>
+  </si>
+  <si>
+    <t>$3FFF-$FFFF = RAM (48 kB)</t>
+  </si>
+  <si>
+    <t>Switch ROM off</t>
+  </si>
+  <si>
+    <t>$0000-$FFFF = RAM (64 kB)</t>
+  </si>
+  <si>
+    <t>Address bit 14 &amp;&amp; 15 == 0 then use ROM</t>
+  </si>
+  <si>
+    <t>Else use RAM</t>
+  </si>
+  <si>
+    <t>If ROM boot is enabled:</t>
+  </si>
+  <si>
+    <r>
+      <t>MEM</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
@@ -772,343 +1753,10 @@
   </si>
   <si>
     <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>c</t>
-    </r>
-  </si>
-  <si>
-    <t>T0</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T8</t>
-  </si>
-  <si>
-    <r>
-      <t>SEQ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>res</t>
-    </r>
-  </si>
-  <si>
-    <t>Load PC into MAR</t>
-  </si>
-  <si>
-    <t>Increment PC</t>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inc</t>
-    </r>
-  </si>
-  <si>
-    <t>Load RAM byte (high) into Y, incr PC</t>
-  </si>
-  <si>
-    <t>Load OpCode from RAM, incr PC</t>
-  </si>
-  <si>
-    <t>Load RAM byte (low) into X, incr PC</t>
-  </si>
-  <si>
-    <t>Load X &amp; Y into MAR</t>
-  </si>
-  <si>
-    <t>Load data from memory location into B and store A + B in A register</t>
-  </si>
-  <si>
-    <t>Load PC into X &amp; Y</t>
-  </si>
-  <si>
-    <t>Decrement PC</t>
-  </si>
-  <si>
-    <t>Load RAM byte (low) into X</t>
-  </si>
-  <si>
-    <t>T9</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>T11</t>
-  </si>
-  <si>
-    <t>T12</t>
-  </si>
-  <si>
-    <t>T13</t>
-  </si>
-  <si>
-    <t>T14</t>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dec</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>STK-in</t>
-    </r>
-  </si>
-  <si>
-    <t>Load Y (high addr) into RAM, incr SP</t>
-  </si>
-  <si>
-    <t>Load SP into MAR</t>
-  </si>
-  <si>
-    <r>
-      <t>STK</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dec</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>STK</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inc</t>
-    </r>
-  </si>
-  <si>
-    <t>Decrement SP</t>
-  </si>
-  <si>
-    <t>Load RAM byte (low) into X, decr SP</t>
-  </si>
-  <si>
-    <t>Load RAM byte (high) into Y</t>
-  </si>
-  <si>
-    <r>
-      <t>CLK</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hlt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>MEM</t>
+    </r>
+    <r>
+      <rPr>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
@@ -1118,578 +1766,13 @@
       </rPr>
       <t>out</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PC-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PC-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>IO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RAM</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RAM</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>IN</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>OUT</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dec</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PC</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>STK</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dec</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>STK</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>incr</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PC-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MAR</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>STK-in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>out</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ALU</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>c</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SEQ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>res</t>
-    </r>
-  </si>
-  <si>
-    <t>Load X (high addr) into RAM, incr SP, decr PC</t>
-  </si>
-  <si>
-    <t>Load X &amp; Y into PC, reset Sequencer</t>
-  </si>
-  <si>
-    <t>ALU Add (A+B), load ALU into A, load Flags, reset Sequencer</t>
-  </si>
-  <si>
-    <t>Load A into RAM, reset Sequencer</t>
-  </si>
-  <si>
-    <t>Load RAM byte into A, reset Sequencer</t>
-  </si>
-  <si>
-    <t>Load RAM byte into A, incr PC, reset SEQ</t>
-  </si>
-  <si>
-    <t>Load A into B, reset Sequencer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1771,6 +1854,14 @@
       <b/>
       <vertAlign val="subscript"/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1858,7 +1949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1941,6 +2032,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2257,7 +2349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5578EEDA-4B03-4105-B303-3E7511EBF0D6}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -2474,7 +2566,7 @@
         <v>30</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F26" s="14"/>
     </row>
@@ -2724,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ECA8DB-9B6A-4777-9CFE-D93FD9D4CCB6}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2735,7 +2827,7 @@
         <v>88</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2743,7 +2835,7 @@
         <v>89</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2751,7 +2843,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2759,7 +2851,7 @@
         <v>91</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2767,7 +2859,7 @@
         <v>92</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2775,7 +2867,7 @@
         <v>93</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2783,7 +2875,7 @@
         <v>94</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2791,7 +2883,7 @@
         <v>95</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2799,7 +2891,7 @@
         <v>96</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2807,7 +2899,7 @@
         <v>97</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2815,7 +2907,7 @@
         <v>98</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2823,7 +2915,7 @@
         <v>99</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.4">
@@ -2831,49 +2923,49 @@
         <v>100</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
-        <v>101</v>
+        <v>221</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -2900,9 +2992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545E2692-A379-484B-9E09-0025D3690B1B}">
   <dimension ref="A1:AL87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -2951,118 +3043,118 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="L1" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="N1" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="P1" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q1" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="S1" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="T1" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="U1" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="V1" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="W1" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="X1" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="W1" s="30" t="s">
+      <c r="Y1" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="Z1" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="AA1" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AB1" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="AA1" s="30" t="s">
+      <c r="AC1" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="31" t="s">
+      <c r="AD1" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AE1" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="AD1" s="31" t="s">
+      <c r="AF1" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="AE1" s="30" t="s">
+      <c r="AG1" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="AF1" s="31" t="s">
+      <c r="AH1" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="AG1" s="30" t="s">
+      <c r="AI1" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="AH1" s="31" t="s">
+      <c r="AJ1" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="AI1" s="30" t="s">
+      <c r="AK1" s="30" t="s">
         <v>185</v>
-      </c>
-      <c r="AJ1" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK1" s="30" t="s">
-        <v>187</v>
       </c>
       <c r="AL1" s="32"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA2" s="22" t="s">
         <v>19</v>
@@ -3070,10 +3162,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>19</v>
@@ -3167,10 +3259,10 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="19"/>
@@ -3296,10 +3388,10 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="19"/>
@@ -3341,10 +3433,10 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>19</v>
@@ -3441,10 +3533,10 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="19"/>
@@ -3486,10 +3578,10 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>19</v>
@@ -3503,10 +3595,10 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA15" s="22" t="s">
         <v>19</v>
@@ -3514,10 +3606,10 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>19</v>
@@ -3531,10 +3623,10 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y17" s="22" t="s">
         <v>19</v>
@@ -3545,10 +3637,10 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>19</v>
@@ -3642,10 +3734,10 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="19"/>
@@ -3687,10 +3779,10 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G22" s="22" t="s">
         <v>19</v>
@@ -3704,10 +3796,10 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA23" s="22" t="s">
         <v>19</v>
@@ -3715,10 +3807,10 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>19</v>
@@ -3732,10 +3824,10 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y25" s="22" t="s">
         <v>19</v>
@@ -3746,10 +3838,10 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K26" s="22" t="s">
         <v>19</v>
@@ -3843,10 +3935,10 @@
     </row>
     <row r="29" spans="1:37" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
@@ -3982,10 +4074,10 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="21"/>
@@ -4027,10 +4119,10 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="19"/>
@@ -4072,10 +4164,10 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="19"/>
@@ -4121,10 +4213,10 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB35" s="16" t="s">
         <v>19</v>
@@ -4132,10 +4224,10 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H36" s="16" t="s">
         <v>19</v>
@@ -4149,10 +4241,10 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB37" s="16" t="s">
         <v>19</v>
@@ -4160,10 +4252,10 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="S38" s="22" t="s">
         <v>19</v>
@@ -4174,10 +4266,10 @@
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S39" s="22" t="s">
         <v>19</v>
@@ -4185,10 +4277,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA40" s="22" t="s">
         <v>19</v>
@@ -4196,10 +4288,10 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G41" s="22" t="s">
         <v>19</v>
@@ -4213,10 +4305,10 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA42" s="22" t="s">
         <v>19</v>
@@ -4224,10 +4316,10 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>19</v>
@@ -4238,10 +4330,10 @@
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U44" s="22" t="s">
         <v>19</v>
@@ -4335,10 +4427,10 @@
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" s="25"/>
       <c r="D47" s="19"/>
@@ -4380,10 +4472,10 @@
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB48" s="16" t="s">
         <v>19</v>
@@ -4391,10 +4483,10 @@
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>19</v>
@@ -4408,10 +4500,10 @@
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB50" s="16" t="s">
         <v>19</v>
@@ -4419,10 +4511,10 @@
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G51" s="22" t="s">
         <v>19</v>
@@ -4433,10 +4525,10 @@
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U52" s="22" t="s">
         <v>19</v>
@@ -4587,6 +4679,177 @@
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDDC48F-A012-4B2D-9E57-CAD8DCD5C18E}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2210CBDD-26D5-4921-9B4C-901277D0D6CF}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added A and B register schematic
</commit_message>
<xml_diff>
--- a/Instructions_T-States.xlsx
+++ b/Instructions_T-States.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Projects\In progress\TTL-computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\TTL-Computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{032618E1-E534-4C4C-A928-851DA9E6DC5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -17,6 +18,7 @@
     <sheet name="T-states" sheetId="3" r:id="rId3"/>
     <sheet name="Notes" sheetId="5" r:id="rId4"/>
     <sheet name="ROM Loader" sheetId="4" r:id="rId5"/>
+    <sheet name="Links" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="252">
   <si>
     <t>Opcode</t>
   </si>
@@ -2649,12 +2651,15 @@
   </si>
   <si>
     <t>Output data from register A (needs to be worked out)</t>
+  </si>
+  <si>
+    <t>http://apollo181.wixsite.com/apollo181/shift-right-with-74181</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3257,27 +3262,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K6:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" style="3" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="24.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="60.5703125" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="40.33203125" style="3" customWidth="1"/>
+    <col min="6" max="9" width="9.109375" style="3"/>
+    <col min="10" max="10" width="24.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3303,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -3312,7 +3317,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -3323,7 +3328,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3334,7 +3339,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3345,7 +3350,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3356,7 +3361,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3383,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -3389,7 +3394,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -3411,7 +3416,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -3422,7 +3427,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -3433,7 +3438,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -3478,7 +3483,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -3492,7 +3497,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -3512,7 +3517,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -3529,7 +3534,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -3546,7 +3551,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -3563,7 +3568,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
@@ -3583,7 +3588,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
@@ -3605,7 +3610,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -3616,7 +3621,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
@@ -3758,7 +3763,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>64</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
         <v>66</v>
       </c>
@@ -3779,7 +3784,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
         <v>67</v>
       </c>
@@ -3792,7 +3797,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>68</v>
       </c>
@@ -3860,16 +3865,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>84</v>
       </c>
@@ -3877,7 +3882,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
@@ -3885,7 +3890,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>86</v>
       </c>
@@ -3893,7 +3898,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>87</v>
       </c>
@@ -3901,7 +3906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>88</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>89</v>
       </c>
@@ -3917,7 +3922,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>90</v>
       </c>
@@ -3925,7 +3930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>91</v>
       </c>
@@ -3933,7 +3938,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>92</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>93</v>
       </c>
@@ -3949,7 +3954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>94</v>
       </c>
@@ -3957,7 +3962,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>95</v>
       </c>
@@ -3965,7 +3970,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>96</v>
       </c>
@@ -3973,7 +3978,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>216</v>
       </c>
@@ -3981,7 +3986,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>97</v>
       </c>
@@ -3989,7 +3994,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>98</v>
       </c>
@@ -3997,37 +4002,37 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
       <c r="C17" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
     </row>
   </sheetData>
@@ -4036,7 +4041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL87"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -4044,49 +4049,49 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
     <col min="2" max="2" width="32" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" style="19" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" style="19" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" style="19" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="5.140625" style="19" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="13" customWidth="1"/>
-    <col min="21" max="21" width="5.140625" style="19" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" style="13" customWidth="1"/>
-    <col min="23" max="23" width="5.140625" style="19" customWidth="1"/>
-    <col min="24" max="24" width="5.140625" style="13" customWidth="1"/>
-    <col min="25" max="25" width="5.140625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="5.140625" style="13" customWidth="1"/>
-    <col min="27" max="27" width="5.140625" style="19" customWidth="1"/>
-    <col min="28" max="28" width="5.140625" style="13" customWidth="1"/>
-    <col min="29" max="29" width="5.140625" style="19" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="13" customWidth="1"/>
-    <col min="31" max="31" width="5.140625" style="19" customWidth="1"/>
-    <col min="32" max="32" width="5.140625" style="13" customWidth="1"/>
-    <col min="33" max="33" width="5.140625" style="19" customWidth="1"/>
-    <col min="34" max="34" width="5.140625" style="13" customWidth="1"/>
-    <col min="35" max="35" width="5.140625" style="19" customWidth="1"/>
-    <col min="36" max="36" width="5.140625" style="13" customWidth="1"/>
-    <col min="37" max="37" width="5.140625" style="19" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="5.109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" style="19" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="5.109375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" style="19" customWidth="1"/>
+    <col min="14" max="14" width="5.109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="19" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" style="19" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" style="13" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" style="19" customWidth="1"/>
+    <col min="20" max="20" width="5.109375" style="13" customWidth="1"/>
+    <col min="21" max="21" width="5.109375" style="19" customWidth="1"/>
+    <col min="22" max="22" width="5.109375" style="13" customWidth="1"/>
+    <col min="23" max="23" width="5.109375" style="19" customWidth="1"/>
+    <col min="24" max="24" width="5.109375" style="13" customWidth="1"/>
+    <col min="25" max="25" width="5.109375" style="19" customWidth="1"/>
+    <col min="26" max="26" width="5.109375" style="13" customWidth="1"/>
+    <col min="27" max="27" width="5.109375" style="19" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" style="13" customWidth="1"/>
+    <col min="29" max="29" width="5.109375" style="19" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="13" customWidth="1"/>
+    <col min="31" max="31" width="5.109375" style="19" customWidth="1"/>
+    <col min="32" max="32" width="5.109375" style="13" customWidth="1"/>
+    <col min="33" max="33" width="5.109375" style="19" customWidth="1"/>
+    <col min="34" max="34" width="5.109375" style="13" customWidth="1"/>
+    <col min="35" max="35" width="5.109375" style="19" customWidth="1"/>
+    <col min="36" max="36" width="5.109375" style="13" customWidth="1"/>
+    <col min="37" max="37" width="5.109375" style="19" customWidth="1"/>
+    <col min="38" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="27" t="s">
@@ -4196,7 +4201,7 @@
       </c>
       <c r="AL1" s="29"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>113</v>
       </c>
@@ -4224,7 +4229,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:38" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="20"/>
@@ -4263,7 +4268,7 @@
       <c r="AJ4" s="14"/>
       <c r="AK4" s="20"/>
     </row>
-    <row r="5" spans="1:38" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -4304,7 +4309,7 @@
       <c r="AJ5" s="15"/>
       <c r="AK5" s="21"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>114</v>
       </c>
@@ -4353,7 +4358,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="23"/>
@@ -4392,7 +4397,7 @@
       <c r="AJ7" s="17"/>
       <c r="AK7" s="23"/>
     </row>
-    <row r="8" spans="1:38" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -4433,7 +4438,7 @@
       <c r="AJ8" s="15"/>
       <c r="AK8" s="21"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>114</v>
       </c>
@@ -4478,7 +4483,7 @@
       <c r="AJ9" s="16"/>
       <c r="AK9" s="22"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>115</v>
       </c>
@@ -4498,7 +4503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="23"/>
@@ -4537,7 +4542,7 @@
       <c r="AJ11" s="17"/>
       <c r="AK11" s="23"/>
     </row>
-    <row r="12" spans="1:38" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -4578,7 +4583,7 @@
       <c r="AJ12" s="15"/>
       <c r="AK12" s="21"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>114</v>
       </c>
@@ -4623,7 +4628,7 @@
       <c r="AJ13" s="16"/>
       <c r="AK13" s="22"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>115</v>
       </c>
@@ -4640,7 +4645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>116</v>
       </c>
@@ -4651,7 +4656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>117</v>
       </c>
@@ -4668,7 +4673,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>118</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>119</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="23"/>
@@ -4738,7 +4743,7 @@
       <c r="AJ19" s="17"/>
       <c r="AK19" s="23"/>
     </row>
-    <row r="20" spans="1:37" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -4779,7 +4784,7 @@
       <c r="AJ20" s="15"/>
       <c r="AK20" s="21"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>114</v>
       </c>
@@ -4824,7 +4829,7 @@
       <c r="AJ21" s="16"/>
       <c r="AK21" s="22"/>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>115</v>
       </c>
@@ -4841,7 +4846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>116</v>
       </c>
@@ -4852,7 +4857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>117</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
@@ -4883,7 +4888,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>119</v>
       </c>
@@ -4900,7 +4905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="23"/>
@@ -4939,7 +4944,7 @@
       <c r="AJ27" s="17"/>
       <c r="AK27" s="23"/>
     </row>
-    <row r="28" spans="1:37" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -4980,7 +4985,7 @@
       <c r="AJ28" s="15"/>
       <c r="AK28" s="21"/>
     </row>
-    <row r="29" spans="1:37" s="36" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" s="36" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>114</v>
       </c>
@@ -5039,7 +5044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="23"/>
@@ -5078,7 +5083,7 @@
       <c r="AJ30" s="17"/>
       <c r="AK30" s="23"/>
     </row>
-    <row r="31" spans="1:37" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -5119,7 +5124,7 @@
       <c r="AJ31" s="15"/>
       <c r="AK31" s="21"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>114</v>
       </c>
@@ -5164,7 +5169,7 @@
       <c r="AJ32" s="18"/>
       <c r="AK32" s="24"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>115</v>
       </c>
@@ -5209,7 +5214,7 @@
       <c r="AJ33" s="16"/>
       <c r="AK33" s="22"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>116</v>
       </c>
@@ -5258,7 +5263,7 @@
       <c r="AJ34" s="16"/>
       <c r="AK34" s="22"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>117</v>
       </c>
@@ -5269,7 +5274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>118</v>
       </c>
@@ -5286,7 +5291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>119</v>
       </c>
@@ -5297,7 +5302,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>120</v>
       </c>
@@ -5311,7 +5316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>132</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>133</v>
       </c>
@@ -5333,7 +5338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>134</v>
       </c>
@@ -5350,7 +5355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>135</v>
       </c>
@@ -5361,7 +5366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>136</v>
       </c>
@@ -5375,7 +5380,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>137</v>
       </c>
@@ -5392,7 +5397,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:37" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="23"/>
@@ -5431,7 +5436,7 @@
       <c r="AJ45" s="17"/>
       <c r="AK45" s="23"/>
     </row>
-    <row r="46" spans="1:37" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -5472,7 +5477,7 @@
       <c r="AJ46" s="15"/>
       <c r="AK46" s="21"/>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>114</v>
       </c>
@@ -5517,7 +5522,7 @@
       <c r="AJ47" s="16"/>
       <c r="AK47" s="22"/>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>115</v>
       </c>
@@ -5528,7 +5533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>116</v>
       </c>
@@ -5545,7 +5550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>117</v>
       </c>
@@ -5556,7 +5561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>118</v>
       </c>
@@ -5570,7 +5575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>119</v>
       </c>
@@ -5587,143 +5592,143 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
     </row>
@@ -5734,60 +5739,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>213</v>
       </c>
@@ -5799,19 +5804,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>188</v>
       </c>
@@ -5820,7 +5825,7 @@
       <c r="D1" s="41"/>
       <c r="E1" s="41"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>189</v>
       </c>
@@ -5829,7 +5834,7 @@
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>190</v>
       </c>
@@ -5842,7 +5847,7 @@
       </c>
       <c r="E3" s="41"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>191</v>
       </c>
@@ -5855,7 +5860,7 @@
       </c>
       <c r="E4" s="41"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>192</v>
       </c>
@@ -5864,7 +5869,7 @@
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>193</v>
       </c>
@@ -5873,7 +5878,7 @@
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
         <v>194</v>
       </c>
@@ -5884,7 +5889,7 @@
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
         <v>195</v>
       </c>
@@ -5895,7 +5900,7 @@
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
         <v>196</v>
       </c>
@@ -5904,7 +5909,7 @@
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
         <v>197</v>
       </c>
@@ -5913,14 +5918,14 @@
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="41"/>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>198</v>
       </c>
@@ -5929,14 +5934,14 @@
       <c r="D12" s="41"/>
       <c r="E12" s="41"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
         <v>199</v>
       </c>
@@ -5945,7 +5950,7 @@
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
         <v>200</v>
       </c>
@@ -5954,14 +5959,14 @@
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="41" t="s">
         <v>205</v>
       </c>
@@ -5970,21 +5975,21 @@
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
       <c r="E18" s="41"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
       <c r="D19" s="41"/>
       <c r="E19" s="41"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
@@ -5994,4 +5999,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C456B90-FD0E-4377-89E3-C2BF46F5C0EE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="66.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>